<commit_message>
mod 10 & lab 2 completed
completed
</commit_message>
<xml_diff>
--- a/data/SnapshotPrivateManufacturingStats2014.xlsx
+++ b/data/SnapshotPrivateManufacturingStats2014.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>avg_weekly_wage</t>
   </si>
@@ -41,12 +41,6 @@
     <t>total_wages_thousands</t>
   </si>
   <si>
-    <t>num_employees_per_thousand_pop</t>
-  </si>
-  <si>
-    <t>num_businesses_per_thousand_pop</t>
-  </si>
-  <si>
     <t>Alabama</t>
   </si>
   <si>
@@ -354,6 +348,15 @@
   </si>
   <si>
     <t>total_wages_dollars_per_100dollars_GDP</t>
+  </si>
+  <si>
+    <t>avg_annual_pay_thousands</t>
+  </si>
+  <si>
+    <t>num_employees_per_tenThousand_pop</t>
+  </si>
+  <si>
+    <t>num_businesses_per_tenThousand_pop</t>
   </si>
 </sst>
 </file>
@@ -705,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,36 +721,36 @@
     <col min="13" max="13" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
@@ -759,18 +762,21 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <f>K2/($I2/10000)</f>
@@ -788,7 +794,8 @@
         <v>1017</v>
       </c>
       <c r="H2">
-        <v>52879</v>
+        <f>O2/1000</f>
+        <v>52.878999999999998</v>
       </c>
       <c r="I2">
         <v>2010453</v>
@@ -809,16 +816,19 @@
         <f>M2/1000</f>
         <v>13368.912</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2">
+        <v>52879</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D49" si="0">K3/($I3/10000)</f>
@@ -836,7 +846,8 @@
         <v>1360</v>
       </c>
       <c r="H3">
-        <v>70718</v>
+        <f t="shared" ref="H3:H49" si="3">O3/1000</f>
+        <v>70.718000000000004</v>
       </c>
       <c r="I3">
         <v>2754982</v>
@@ -854,19 +865,22 @@
         <v>11038257</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N49" si="3">M3/1000</f>
+        <f t="shared" ref="N3:N49" si="4">M3/1000</f>
         <v>11038.257</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3">
+        <v>70718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -884,7 +898,8 @@
         <v>847</v>
       </c>
       <c r="H4">
-        <v>44024</v>
+        <f t="shared" si="3"/>
+        <v>44.024000000000001</v>
       </c>
       <c r="I4">
         <v>1251717</v>
@@ -902,19 +917,22 @@
         <v>6785328</v>
       </c>
       <c r="N4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6785.3280000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4">
+        <v>44024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -932,7 +950,8 @@
         <v>1565</v>
       </c>
       <c r="H5">
-        <v>81368</v>
+        <f t="shared" si="3"/>
+        <v>81.367999999999995</v>
       </c>
       <c r="I5">
         <v>16890442</v>
@@ -950,19 +969,22 @@
         <v>102858859</v>
       </c>
       <c r="N5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102858.859</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>81368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -980,7 +1002,8 @@
         <v>1253</v>
       </c>
       <c r="H6">
-        <v>65168</v>
+        <f t="shared" si="3"/>
+        <v>65.168000000000006</v>
       </c>
       <c r="I6">
         <v>2560703</v>
@@ -998,19 +1021,22 @@
         <v>8876464</v>
       </c>
       <c r="N6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8876.4639999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6">
+        <v>65168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -1028,7 +1054,8 @@
         <v>1565</v>
       </c>
       <c r="H7">
-        <v>81393</v>
+        <f t="shared" si="3"/>
+        <v>81.393000000000001</v>
       </c>
       <c r="I7">
         <v>1766934</v>
@@ -1046,19 +1073,22 @@
         <v>12990893</v>
       </c>
       <c r="N7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12990.893</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O7">
+        <v>81393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -1076,7 +1106,8 @@
         <v>1146</v>
       </c>
       <c r="H8">
-        <v>59588</v>
+        <f t="shared" si="3"/>
+        <v>59.588000000000001</v>
       </c>
       <c r="I8">
         <v>426103</v>
@@ -1094,19 +1125,22 @@
         <v>1529719</v>
       </c>
       <c r="N8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1529.7190000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O8">
+        <v>59588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -1124,7 +1158,8 @@
         <v>1068</v>
       </c>
       <c r="H9">
-        <v>55517</v>
+        <f t="shared" si="3"/>
+        <v>55.517000000000003</v>
       </c>
       <c r="I9">
         <v>8335023</v>
@@ -1142,19 +1177,22 @@
         <v>18379505</v>
       </c>
       <c r="N9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18379.505000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O9">
+        <v>55517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -1172,7 +1210,8 @@
         <v>1061</v>
       </c>
       <c r="H10">
-        <v>55151</v>
+        <f t="shared" si="3"/>
+        <v>55.151000000000003</v>
       </c>
       <c r="I10">
         <v>4300074</v>
@@ -1190,19 +1229,22 @@
         <v>20115436</v>
       </c>
       <c r="N10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20115.436000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O10">
+        <v>55151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -1220,7 +1262,8 @@
         <v>1123</v>
       </c>
       <c r="H11">
-        <v>58409</v>
+        <f t="shared" si="3"/>
+        <v>58.408999999999999</v>
       </c>
       <c r="I11">
         <v>703410</v>
@@ -1238,19 +1281,22 @@
         <v>3496913</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3496.913</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O11">
+        <v>58409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -1268,7 +1314,8 @@
         <v>1267</v>
       </c>
       <c r="H12">
-        <v>65866</v>
+        <f t="shared" si="3"/>
+        <v>65.866</v>
       </c>
       <c r="I12">
         <v>6032031</v>
@@ -1286,19 +1333,22 @@
         <v>38125799</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38125.798999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O12">
+        <v>65866</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -1316,7 +1366,8 @@
         <v>1109</v>
       </c>
       <c r="H13">
-        <v>57667</v>
+        <f t="shared" si="3"/>
+        <v>57.667000000000002</v>
       </c>
       <c r="I13">
         <v>2994736</v>
@@ -1334,19 +1385,22 @@
         <v>29247955</v>
       </c>
       <c r="N13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29247.955000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O13">
+        <v>57667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -1364,7 +1418,8 @@
         <v>1046</v>
       </c>
       <c r="H14">
-        <v>54417</v>
+        <f t="shared" si="3"/>
+        <v>54.417000000000002</v>
       </c>
       <c r="I14">
         <v>1562492</v>
@@ -1382,19 +1437,22 @@
         <v>11800576</v>
       </c>
       <c r="N14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11800.575999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14">
+        <v>54417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -1412,7 +1470,8 @@
         <v>1030</v>
       </c>
       <c r="H15">
-        <v>53558</v>
+        <f t="shared" si="3"/>
+        <v>53.558</v>
       </c>
       <c r="I15">
         <v>1391836</v>
@@ -1430,19 +1489,22 @@
         <v>8697256</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8697.2559999999994</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O15">
+        <v>53558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -1460,7 +1522,8 @@
         <v>1059</v>
       </c>
       <c r="H16">
-        <v>55091</v>
+        <f t="shared" si="3"/>
+        <v>55.091000000000001</v>
       </c>
       <c r="I16">
         <v>1870879</v>
@@ -1478,19 +1541,22 @@
         <v>12927472</v>
       </c>
       <c r="N16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12927.472</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O16">
+        <v>55091</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17">
         <f>K17/($I17/10000)</f>
@@ -1508,7 +1574,8 @@
         <v>1297</v>
       </c>
       <c r="H17">
-        <v>67469</v>
+        <f t="shared" si="3"/>
+        <v>67.468999999999994</v>
       </c>
       <c r="I17">
         <v>2002410</v>
@@ -1526,19 +1593,22 @@
         <v>9924521</v>
       </c>
       <c r="N17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9924.5210000000006</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O17">
+        <v>67469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -1556,7 +1626,8 @@
         <v>1013</v>
       </c>
       <c r="H18">
-        <v>52651</v>
+        <f t="shared" si="3"/>
+        <v>52.651000000000003</v>
       </c>
       <c r="I18">
         <v>646438</v>
@@ -1574,19 +1645,22 @@
         <v>2641678</v>
       </c>
       <c r="N18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2641.6779999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O18">
+        <v>52651</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -1604,7 +1678,8 @@
         <v>1353</v>
       </c>
       <c r="H19">
-        <v>70354</v>
+        <f t="shared" si="3"/>
+        <v>70.353999999999999</v>
       </c>
       <c r="I19">
         <v>2949440</v>
@@ -1622,19 +1697,22 @@
         <v>7276759</v>
       </c>
       <c r="N19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7276.759</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O19">
+        <v>70354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -1652,7 +1730,8 @@
         <v>1604</v>
       </c>
       <c r="H20">
-        <v>83404</v>
+        <f t="shared" si="3"/>
+        <v>83.403999999999996</v>
       </c>
       <c r="I20">
         <v>3354036</v>
@@ -1670,19 +1749,22 @@
         <v>20875989</v>
       </c>
       <c r="N20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20875.989000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O20">
+        <v>83404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -1700,7 +1782,8 @@
         <v>1240</v>
       </c>
       <c r="H21">
-        <v>64469</v>
+        <f t="shared" si="3"/>
+        <v>64.468999999999994</v>
       </c>
       <c r="I21">
         <v>4293574</v>
@@ -1718,19 +1801,22 @@
         <v>37171042</v>
       </c>
       <c r="N21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37171.042000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O21">
+        <v>64469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -1748,7 +1834,8 @@
         <v>1175</v>
       </c>
       <c r="H22">
-        <v>61093</v>
+        <f t="shared" si="3"/>
+        <v>61.093000000000004</v>
       </c>
       <c r="I22">
         <v>2781933</v>
@@ -1766,19 +1853,22 @@
         <v>19054671</v>
       </c>
       <c r="N22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19054.670999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O22">
+        <v>61093</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
@@ -1796,7 +1886,8 @@
         <v>878</v>
       </c>
       <c r="H23">
-        <v>45667</v>
+        <f t="shared" si="3"/>
+        <v>45.667000000000002</v>
       </c>
       <c r="I23">
         <v>1198828</v>
@@ -1814,19 +1905,22 @@
         <v>6372093</v>
       </c>
       <c r="N23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6372.0929999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O23">
+        <v>45667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -1844,7 +1938,8 @@
         <v>1059</v>
       </c>
       <c r="H24">
-        <v>55091</v>
+        <f t="shared" si="3"/>
+        <v>55.091000000000001</v>
       </c>
       <c r="I24">
         <v>2779991</v>
@@ -1862,19 +1957,22 @@
         <v>14099502</v>
       </c>
       <c r="N24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14099.502</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O24">
+        <v>55091</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -1892,7 +1990,8 @@
         <v>879</v>
       </c>
       <c r="H25">
-        <v>45726</v>
+        <f t="shared" si="3"/>
+        <v>45.725999999999999</v>
       </c>
       <c r="I25">
         <v>481119</v>
@@ -1910,19 +2009,22 @@
         <v>863271</v>
       </c>
       <c r="N25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>863.27099999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O25">
+        <v>45726</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -1940,7 +2042,8 @@
         <v>880</v>
       </c>
       <c r="H26">
-        <v>45779</v>
+        <f t="shared" si="3"/>
+        <v>45.779000000000003</v>
       </c>
       <c r="I26">
         <v>957508</v>
@@ -1958,19 +2061,22 @@
         <v>4459847</v>
       </c>
       <c r="N26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4459.8469999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O26">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
@@ -1988,7 +2094,8 @@
         <v>1053</v>
       </c>
       <c r="H27">
-        <v>54734</v>
+        <f t="shared" si="3"/>
+        <v>54.734000000000002</v>
       </c>
       <c r="I27">
         <v>1240614</v>
@@ -2006,19 +2113,22 @@
         <v>2269054</v>
       </c>
       <c r="N27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2269.0540000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O27">
+        <v>54734</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
@@ -2036,7 +2146,8 @@
         <v>1274</v>
       </c>
       <c r="H28">
-        <v>66235</v>
+        <f t="shared" si="3"/>
+        <v>66.234999999999999</v>
       </c>
       <c r="I28">
         <v>693329</v>
@@ -2054,19 +2165,22 @@
         <v>4401359</v>
       </c>
       <c r="N28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4401.3590000000004</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O28">
+        <v>66235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
@@ -2084,7 +2198,8 @@
         <v>1538</v>
       </c>
       <c r="H29">
-        <v>79988</v>
+        <f t="shared" si="3"/>
+        <v>79.988</v>
       </c>
       <c r="I29">
         <v>4235089</v>
@@ -2102,19 +2217,22 @@
         <v>19220478</v>
       </c>
       <c r="N29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19220.477999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O29">
+        <v>79988</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
@@ -2132,7 +2250,8 @@
         <v>1100</v>
       </c>
       <c r="H30">
-        <v>57223</v>
+        <f t="shared" si="3"/>
+        <v>57.222999999999999</v>
       </c>
       <c r="I30">
         <v>875947</v>
@@ -2150,19 +2269,22 @@
         <v>1601206</v>
       </c>
       <c r="N30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1601.2059999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O30">
+        <v>57223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
@@ -2180,7 +2302,8 @@
         <v>1195</v>
       </c>
       <c r="H31">
-        <v>62166</v>
+        <f t="shared" si="3"/>
+        <v>62.165999999999997</v>
       </c>
       <c r="I31">
         <v>9137540</v>
@@ -2198,19 +2321,22 @@
         <v>27988466</v>
       </c>
       <c r="N31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27988.466</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O31">
+        <v>62166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
@@ -2228,7 +2354,8 @@
         <v>1062</v>
       </c>
       <c r="H32">
-        <v>55208</v>
+        <f t="shared" si="3"/>
+        <v>55.207999999999998</v>
       </c>
       <c r="I32">
         <v>4287690</v>
@@ -2246,19 +2373,22 @@
         <v>24772426</v>
       </c>
       <c r="N32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24772.425999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O32">
+        <v>55208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
@@ -2276,7 +2406,8 @@
         <v>957</v>
       </c>
       <c r="H33">
-        <v>49761</v>
+        <f t="shared" si="3"/>
+        <v>49.761000000000003</v>
       </c>
       <c r="I33">
         <v>379972</v>
@@ -2294,19 +2425,22 @@
         <v>1290656</v>
       </c>
       <c r="N33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1290.6559999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O33">
+        <v>49761</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
@@ -2324,7 +2458,8 @@
         <v>1105</v>
       </c>
       <c r="H34">
-        <v>57485</v>
+        <f t="shared" si="3"/>
+        <v>57.484999999999999</v>
       </c>
       <c r="I34">
         <v>5303013</v>
@@ -2342,19 +2477,22 @@
         <v>38757784</v>
       </c>
       <c r="N34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38757.784</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O34">
+        <v>57485</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
@@ -2372,7 +2510,8 @@
         <v>1031</v>
       </c>
       <c r="H35">
-        <v>53621</v>
+        <f t="shared" si="3"/>
+        <v>53.621000000000002</v>
       </c>
       <c r="I35">
         <v>1699610</v>
@@ -2390,19 +2529,22 @@
         <v>7469378</v>
       </c>
       <c r="N35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7469.3779999999997</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O35">
+        <v>53621</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
@@ -2420,7 +2562,8 @@
         <v>1231</v>
       </c>
       <c r="H36">
-        <v>64011</v>
+        <f t="shared" si="3"/>
+        <v>64.010999999999996</v>
       </c>
       <c r="I36">
         <v>1752414</v>
@@ -2438,19 +2581,22 @@
         <v>11461762</v>
       </c>
       <c r="N36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11461.762000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O36">
+        <v>64011</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
@@ -2468,7 +2614,8 @@
         <v>1126</v>
       </c>
       <c r="H37">
-        <v>58553</v>
+        <f t="shared" si="3"/>
+        <v>58.552999999999997</v>
       </c>
       <c r="I37">
         <v>5946480</v>
@@ -2486,19 +2633,22 @@
         <v>33209866</v>
       </c>
       <c r="N37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33209.866000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O37">
+        <v>58553</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
@@ -2516,7 +2666,8 @@
         <v>1052</v>
       </c>
       <c r="H38">
-        <v>54700</v>
+        <f t="shared" si="3"/>
+        <v>54.7</v>
       </c>
       <c r="I38">
         <v>511362</v>
@@ -2534,19 +2685,22 @@
         <v>2232859</v>
       </c>
       <c r="N38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2232.8589999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O38">
+        <v>54700</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
@@ -2564,7 +2718,8 @@
         <v>1063</v>
       </c>
       <c r="H39">
-        <v>55270</v>
+        <f t="shared" si="3"/>
+        <v>55.27</v>
       </c>
       <c r="I39">
         <v>2031997</v>
@@ -2582,19 +2737,22 @@
         <v>12720588</v>
       </c>
       <c r="N39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12720.588</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O39">
+        <v>55270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
@@ -2612,7 +2770,8 @@
         <v>856</v>
       </c>
       <c r="H40">
-        <v>44503</v>
+        <f t="shared" si="3"/>
+        <v>44.503</v>
       </c>
       <c r="I40">
         <v>425816</v>
@@ -2630,19 +2789,22 @@
         <v>1886462</v>
       </c>
       <c r="N40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1886.462</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O40">
+        <v>44503</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
@@ -2660,7 +2822,8 @@
         <v>1083</v>
       </c>
       <c r="H41">
-        <v>56311</v>
+        <f t="shared" si="3"/>
+        <v>56.311</v>
       </c>
       <c r="I41">
         <v>2835895</v>
@@ -2678,19 +2841,22 @@
         <v>18291746</v>
       </c>
       <c r="N41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18291.745999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O41">
+        <v>56311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
@@ -2708,7 +2874,8 @@
         <v>1369</v>
       </c>
       <c r="H42">
-        <v>71189</v>
+        <f t="shared" si="3"/>
+        <v>71.188999999999993</v>
       </c>
       <c r="I42">
         <v>11809010</v>
@@ -2726,19 +2893,22 @@
         <v>63129005</v>
       </c>
       <c r="N42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>63129.004999999997</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O42">
+        <v>71189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
@@ -2756,7 +2926,8 @@
         <v>1018</v>
       </c>
       <c r="H43">
-        <v>52923</v>
+        <f t="shared" si="3"/>
+        <v>52.923000000000002</v>
       </c>
       <c r="I43">
         <v>1299818</v>
@@ -2774,19 +2945,22 @@
         <v>6342506</v>
       </c>
       <c r="N43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6342.5060000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O43">
+        <v>52923</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
@@ -2804,7 +2978,8 @@
         <v>1063</v>
       </c>
       <c r="H44">
-        <v>55290</v>
+        <f t="shared" si="3"/>
+        <v>55.29</v>
       </c>
       <c r="I44">
         <v>325336</v>
@@ -2822,19 +2997,22 @@
         <v>1725075</v>
       </c>
       <c r="N44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1725.075</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O44">
+        <v>55290</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
@@ -2852,7 +3030,8 @@
         <v>1086</v>
       </c>
       <c r="H45">
-        <v>56469</v>
+        <f t="shared" si="3"/>
+        <v>56.469000000000001</v>
       </c>
       <c r="I45">
         <v>3936638</v>
@@ -2870,19 +3049,22 @@
         <v>13068126</v>
       </c>
       <c r="N45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13068.126</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O45">
+        <v>56469</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
@@ -2900,7 +3082,8 @@
         <v>1429</v>
       </c>
       <c r="H46">
-        <v>74328</v>
+        <f t="shared" si="3"/>
+        <v>74.328000000000003</v>
       </c>
       <c r="I46">
         <v>3194382</v>
@@ -2918,19 +3101,22 @@
         <v>21209680</v>
       </c>
       <c r="N46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21209.68</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O46">
+        <v>74328</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
@@ -2948,7 +3134,8 @@
         <v>1058</v>
       </c>
       <c r="H47">
-        <v>55017</v>
+        <f t="shared" si="3"/>
+        <v>55.017000000000003</v>
       </c>
       <c r="I47">
         <v>753227</v>
@@ -2966,19 +3153,22 @@
         <v>2628371</v>
       </c>
       <c r="N47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2628.3710000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O47">
+        <v>55017</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
@@ -2996,7 +3186,8 @@
         <v>1046</v>
       </c>
       <c r="H48">
-        <v>54370</v>
+        <f t="shared" si="3"/>
+        <v>54.37</v>
       </c>
       <c r="I48">
         <v>2852018</v>
@@ -3014,19 +3205,22 @@
         <v>25040119</v>
       </c>
       <c r="N48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25040.118999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O48">
+        <v>54370</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
@@ -3044,7 +3238,8 @@
         <v>1165</v>
       </c>
       <c r="H49">
-        <v>60562</v>
+        <f t="shared" si="3"/>
+        <v>60.561999999999998</v>
       </c>
       <c r="I49">
         <v>291552</v>
@@ -3062,8 +3257,11 @@
         <v>594217</v>
       </c>
       <c r="N49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>594.21699999999998</v>
+      </c>
+      <c r="O49">
+        <v>60562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>